<commit_message>
major update of correction files
</commit_message>
<xml_diff>
--- a/in/extraction1/corrections/supp_CR.xlsx
+++ b/in/extraction1/corrections/supp_CR.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Code sexe</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>ZD</t>
+  </si>
+  <si>
+    <t>04</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -630,6 +633,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -953,11 +962,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -992,7 +1003,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="10" t="s">
@@ -1057,8 +1068,8 @@
       </c>
     </row>
     <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
+      <c r="A2" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -1122,7 +1133,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="13"/>
       <c r="E3" s="4"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -1130,7 +1141,7 @@
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="13"/>
       <c r="E4" s="4"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -1138,7 +1149,7 @@
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="13"/>
       <c r="E5" s="4"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -1147,7 +1158,7 @@
       <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="13"/>
       <c r="E6" s="4"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -1156,21 +1167,21 @@
       <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="13"/>
       <c r="E7" s="4"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="13"/>
       <c r="E8" s="4"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="13"/>
       <c r="E9" s="4"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1179,14 +1190,14 @@
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="13"/>
       <c r="E10" s="4"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="13"/>
       <c r="E11" s="4"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -1194,7 +1205,7 @@
       <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="13"/>
       <c r="E12" s="4"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -1203,7 +1214,7 @@
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="13"/>
       <c r="E13" s="4"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -1211,7 +1222,7 @@
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="13"/>
       <c r="E14" s="4"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1220,7 +1231,7 @@
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="13"/>
       <c r="E15" s="4"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1228,7 +1239,7 @@
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="13"/>
       <c r="E16" s="4"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
@@ -1237,14 +1248,14 @@
       <c r="P16" s="9"/>
     </row>
     <row r="17" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="13"/>
       <c r="E17" s="4"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="13"/>
       <c r="E18" s="4"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
@@ -1253,21 +1264,21 @@
       <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="13"/>
       <c r="E19" s="4"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="13"/>
       <c r="E20" s="4"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="13"/>
       <c r="E21" s="4"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -1276,7 +1287,7 @@
       <c r="P21" s="9"/>
     </row>
     <row r="22" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="13"/>
       <c r="E22" s="4"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -1285,7 +1296,7 @@
       <c r="P22" s="9"/>
     </row>
     <row r="23" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="13"/>
       <c r="E23" s="4"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -1294,14 +1305,14 @@
       <c r="P23" s="9"/>
     </row>
     <row r="24" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="13"/>
       <c r="E24" s="4"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="13"/>
       <c r="E25" s="4"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1310,14 +1321,14 @@
       <c r="P25" s="9"/>
     </row>
     <row r="26" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="13"/>
       <c r="E26" s="4"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="N26" s="7"/>
     </row>
     <row r="27" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+      <c r="A27" s="13"/>
       <c r="E27" s="4"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -1326,7 +1337,7 @@
       <c r="P27" s="9"/>
     </row>
     <row r="28" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+      <c r="A28" s="13"/>
       <c r="E28" s="4"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
@@ -1335,7 +1346,7 @@
       <c r="P28" s="9"/>
     </row>
     <row r="29" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+      <c r="A29" s="13"/>
       <c r="E29" s="4"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1343,7 +1354,7 @@
       <c r="O29" s="9"/>
     </row>
     <row r="30" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="13"/>
       <c r="E30" s="4"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
@@ -1352,21 +1363,21 @@
       <c r="P30" s="9"/>
     </row>
     <row r="31" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+      <c r="A31" s="13"/>
       <c r="E31" s="4"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="N31" s="7"/>
     </row>
     <row r="32" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="13"/>
       <c r="E32" s="4"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="N32" s="7"/>
     </row>
     <row r="33" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="13"/>
       <c r="E33" s="4"/>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -1375,7 +1386,7 @@
       <c r="P33" s="9"/>
     </row>
     <row r="34" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="13"/>
       <c r="E34" s="4"/>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -1384,7 +1395,7 @@
       <c r="P34" s="9"/>
     </row>
     <row r="35" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="13"/>
       <c r="E35" s="4"/>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -1393,7 +1404,7 @@
       <c r="P35" s="9"/>
     </row>
     <row r="36" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="13"/>
       <c r="E36" s="4"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -1402,28 +1413,28 @@
       <c r="P36" s="9"/>
     </row>
     <row r="37" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
+      <c r="A37" s="13"/>
       <c r="E37" s="4"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
       <c r="N37" s="7"/>
     </row>
     <row r="38" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
+      <c r="A38" s="13"/>
       <c r="E38" s="4"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="N38" s="7"/>
     </row>
     <row r="39" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
+      <c r="A39" s="13"/>
       <c r="E39" s="4"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="N39" s="7"/>
     </row>
     <row r="40" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+      <c r="A40" s="13"/>
       <c r="E40" s="4"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
@@ -1432,7 +1443,7 @@
       <c r="P40" s="9"/>
     </row>
     <row r="41" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
+      <c r="A41" s="13"/>
       <c r="E41" s="4"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
@@ -1441,7 +1452,7 @@
       <c r="P41" s="9"/>
     </row>
     <row r="42" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="13"/>
       <c r="E42" s="4"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
@@ -1450,7 +1461,7 @@
       <c r="P42" s="9"/>
     </row>
     <row r="43" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
+      <c r="A43" s="13"/>
       <c r="E43" s="4"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
@@ -1458,7 +1469,7 @@
       <c r="O43" s="9"/>
     </row>
     <row r="44" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
+      <c r="A44" s="13"/>
       <c r="E44" s="4"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -1467,7 +1478,7 @@
       <c r="P44" s="9"/>
     </row>
     <row r="45" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
+      <c r="A45" s="13"/>
       <c r="E45" s="4"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -1475,28 +1486,28 @@
       <c r="O45" s="9"/>
     </row>
     <row r="46" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
+      <c r="A46" s="13"/>
       <c r="E46" s="4"/>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="N46" s="7"/>
     </row>
     <row r="47" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
+      <c r="A47" s="13"/>
       <c r="E47" s="4"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="N47" s="7"/>
     </row>
     <row r="48" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
+      <c r="A48" s="13"/>
       <c r="E48" s="4"/>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="N48" s="7"/>
     </row>
     <row r="49" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="13"/>
       <c r="E49" s="4"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -1504,14 +1515,14 @@
       <c r="O49" s="9"/>
     </row>
     <row r="50" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
+      <c r="A50" s="13"/>
       <c r="E50" s="4"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="N50" s="7"/>
     </row>
     <row r="51" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
+      <c r="A51" s="13"/>
       <c r="E51" s="4"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -1519,7 +1530,7 @@
       <c r="O51" s="9"/>
     </row>
     <row r="52" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
+      <c r="A52" s="13"/>
       <c r="E52" s="4"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -1528,21 +1539,21 @@
       <c r="P52" s="9"/>
     </row>
     <row r="53" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
+      <c r="A53" s="13"/>
       <c r="E53" s="4"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="N53" s="7"/>
     </row>
     <row r="54" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
+      <c r="A54" s="13"/>
       <c r="E54" s="4"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="N54" s="7"/>
     </row>
     <row r="55" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
+      <c r="A55" s="13"/>
       <c r="E55" s="4"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -1551,7 +1562,7 @@
       <c r="P55" s="9"/>
     </row>
     <row r="56" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
+      <c r="A56" s="13"/>
       <c r="E56" s="4"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -1560,7 +1571,7 @@
       <c r="P56" s="9"/>
     </row>
     <row r="57" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
+      <c r="A57" s="13"/>
       <c r="E57" s="4"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -1569,7 +1580,7 @@
       <c r="P57" s="9"/>
     </row>
     <row r="58" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
+      <c r="A58" s="13"/>
       <c r="E58" s="4"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -1578,7 +1589,7 @@
       <c r="P58" s="9"/>
     </row>
     <row r="59" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
+      <c r="A59" s="13"/>
       <c r="E59" s="4"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -1587,7 +1598,7 @@
       <c r="P59" s="9"/>
     </row>
     <row r="60" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
+      <c r="A60" s="13"/>
       <c r="E60" s="4"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -1596,7 +1607,7 @@
       <c r="P60" s="9"/>
     </row>
     <row r="61" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
+      <c r="A61" s="13"/>
       <c r="E61" s="4"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -1605,7 +1616,7 @@
       <c r="P61" s="9"/>
     </row>
     <row r="62" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
+      <c r="A62" s="13"/>
       <c r="E62" s="4"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -1614,35 +1625,35 @@
       <c r="P62" s="9"/>
     </row>
     <row r="63" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
+      <c r="A63" s="13"/>
       <c r="E63" s="4"/>
       <c r="J63" s="6"/>
       <c r="K63" s="6"/>
       <c r="N63" s="7"/>
     </row>
     <row r="64" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
+      <c r="A64" s="13"/>
       <c r="E64" s="4"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
       <c r="N64" s="7"/>
     </row>
     <row r="65" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
+      <c r="A65" s="13"/>
       <c r="E65" s="4"/>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
       <c r="N65" s="7"/>
     </row>
     <row r="66" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
+      <c r="A66" s="13"/>
       <c r="E66" s="4"/>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
       <c r="N66" s="7"/>
     </row>
     <row r="67" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
+      <c r="A67" s="13"/>
       <c r="E67" s="4"/>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
@@ -1651,7 +1662,7 @@
       <c r="P67" s="9"/>
     </row>
     <row r="68" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
+      <c r="A68" s="13"/>
       <c r="E68" s="4"/>
       <c r="J68" s="6"/>
       <c r="K68" s="6"/>
@@ -1660,14 +1671,14 @@
       <c r="P68" s="9"/>
     </row>
     <row r="69" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
+      <c r="A69" s="13"/>
       <c r="E69" s="4"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
       <c r="N69" s="7"/>
     </row>
     <row r="70" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
+      <c r="A70" s="13"/>
       <c r="E70" s="4"/>
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
@@ -1676,7 +1687,7 @@
       <c r="P70" s="9"/>
     </row>
     <row r="71" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
+      <c r="A71" s="13"/>
       <c r="E71" s="4"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
@@ -1685,14 +1696,14 @@
       <c r="P71" s="9"/>
     </row>
     <row r="72" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
+      <c r="A72" s="13"/>
       <c r="E72" s="4"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="N72" s="7"/>
     </row>
     <row r="73" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
+      <c r="A73" s="13"/>
       <c r="E73" s="4"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
@@ -1700,7 +1711,7 @@
       <c r="O73" s="9"/>
     </row>
     <row r="74" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
+      <c r="A74" s="13"/>
       <c r="E74" s="4"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
@@ -1708,7 +1719,7 @@
       <c r="O74" s="9"/>
     </row>
     <row r="75" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
+      <c r="A75" s="13"/>
       <c r="E75" s="4"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
@@ -1717,7 +1728,7 @@
       <c r="P75" s="9"/>
     </row>
     <row r="76" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
+      <c r="A76" s="13"/>
       <c r="E76" s="4"/>
       <c r="J76" s="6"/>
       <c r="K76" s="6"/>
@@ -1726,21 +1737,21 @@
       <c r="P76" s="9"/>
     </row>
     <row r="77" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
+      <c r="A77" s="13"/>
       <c r="E77" s="4"/>
       <c r="J77" s="6"/>
       <c r="K77" s="6"/>
       <c r="N77" s="7"/>
     </row>
     <row r="78" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
+      <c r="A78" s="13"/>
       <c r="E78" s="4"/>
       <c r="J78" s="6"/>
       <c r="K78" s="6"/>
       <c r="N78" s="7"/>
     </row>
     <row r="79" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
+      <c r="A79" s="13"/>
       <c r="E79" s="4"/>
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
@@ -1749,14 +1760,14 @@
       <c r="P79" s="9"/>
     </row>
     <row r="80" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
+      <c r="A80" s="13"/>
       <c r="E80" s="4"/>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
       <c r="N80" s="7"/>
     </row>
     <row r="81" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
+      <c r="A81" s="13"/>
       <c r="E81" s="4"/>
       <c r="J81" s="6"/>
       <c r="K81" s="6"/>
@@ -1765,7 +1776,7 @@
       <c r="P81" s="9"/>
     </row>
     <row r="82" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
+      <c r="A82" s="13"/>
       <c r="E82" s="4"/>
       <c r="J82" s="6"/>
       <c r="K82" s="6"/>
@@ -1774,7 +1785,7 @@
       <c r="P82" s="9"/>
     </row>
     <row r="83" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
+      <c r="A83" s="13"/>
       <c r="E83" s="4"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
@@ -1782,21 +1793,21 @@
       <c r="O83" s="9"/>
     </row>
     <row r="84" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
+      <c r="A84" s="13"/>
       <c r="E84" s="4"/>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
       <c r="N84" s="7"/>
     </row>
     <row r="85" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
+      <c r="A85" s="13"/>
       <c r="E85" s="4"/>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
       <c r="N85" s="7"/>
     </row>
     <row r="86" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
+      <c r="A86" s="13"/>
       <c r="E86" s="4"/>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -1804,14 +1815,14 @@
       <c r="O86" s="9"/>
     </row>
     <row r="87" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
+      <c r="A87" s="13"/>
       <c r="E87" s="4"/>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
       <c r="N87" s="7"/>
     </row>
     <row r="88" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
+      <c r="A88" s="13"/>
       <c r="E88" s="4"/>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -1820,7 +1831,7 @@
       <c r="P88" s="9"/>
     </row>
     <row r="89" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
+      <c r="A89" s="13"/>
       <c r="E89" s="4"/>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -1829,7 +1840,7 @@
       <c r="P89" s="9"/>
     </row>
     <row r="90" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
+      <c r="A90" s="13"/>
       <c r="E90" s="4"/>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
@@ -1838,21 +1849,21 @@
       <c r="P90" s="9"/>
     </row>
     <row r="91" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
+      <c r="A91" s="13"/>
       <c r="E91" s="4"/>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
       <c r="N91" s="7"/>
     </row>
     <row r="92" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
+      <c r="A92" s="13"/>
       <c r="E92" s="4"/>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
       <c r="N92" s="7"/>
     </row>
     <row r="93" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
+      <c r="A93" s="13"/>
       <c r="E93" s="4"/>
       <c r="J93" s="6"/>
       <c r="K93" s="6"/>
@@ -1861,7 +1872,7 @@
       <c r="P93" s="9"/>
     </row>
     <row r="94" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
+      <c r="A94" s="13"/>
       <c r="E94" s="4"/>
       <c r="J94" s="6"/>
       <c r="K94" s="6"/>
@@ -1870,7 +1881,7 @@
       <c r="P94" s="9"/>
     </row>
     <row r="95" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
+      <c r="A95" s="13"/>
       <c r="E95" s="4"/>
       <c r="J95" s="6"/>
       <c r="K95" s="6"/>
@@ -1879,7 +1890,7 @@
       <c r="P95" s="9"/>
     </row>
     <row r="96" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
+      <c r="A96" s="13"/>
       <c r="E96" s="4"/>
       <c r="J96" s="6"/>
       <c r="K96" s="6"/>
@@ -1888,14 +1899,14 @@
       <c r="P96" s="9"/>
     </row>
     <row r="97" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
+      <c r="A97" s="13"/>
       <c r="E97" s="4"/>
       <c r="J97" s="6"/>
       <c r="K97" s="6"/>
       <c r="N97" s="7"/>
     </row>
     <row r="98" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
+      <c r="A98" s="13"/>
       <c r="E98" s="4"/>
       <c r="J98" s="6"/>
       <c r="K98" s="6"/>
@@ -1904,7 +1915,7 @@
       <c r="P98" s="9"/>
     </row>
     <row r="99" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
+      <c r="A99" s="13"/>
       <c r="E99" s="4"/>
       <c r="J99" s="6"/>
       <c r="K99" s="6"/>
@@ -1913,14 +1924,14 @@
       <c r="P99" s="9"/>
     </row>
     <row r="100" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
+      <c r="A100" s="13"/>
       <c r="E100" s="4"/>
       <c r="J100" s="6"/>
       <c r="K100" s="6"/>
       <c r="N100" s="7"/>
     </row>
     <row r="101" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
+      <c r="A101" s="13"/>
       <c r="E101" s="4"/>
       <c r="J101" s="6"/>
       <c r="K101" s="6"/>
@@ -1928,7 +1939,7 @@
       <c r="O101" s="9"/>
     </row>
     <row r="102" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4"/>
+      <c r="A102" s="13"/>
       <c r="E102" s="4"/>
       <c r="J102" s="6"/>
       <c r="K102" s="6"/>
@@ -1937,7 +1948,7 @@
       <c r="P102" s="9"/>
     </row>
     <row r="103" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
+      <c r="A103" s="13"/>
       <c r="E103" s="4"/>
       <c r="J103" s="6"/>
       <c r="K103" s="6"/>
@@ -1945,14 +1956,14 @@
       <c r="O103" s="9"/>
     </row>
     <row r="104" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
+      <c r="A104" s="13"/>
       <c r="E104" s="4"/>
       <c r="J104" s="6"/>
       <c r="K104" s="6"/>
       <c r="N104" s="7"/>
     </row>
     <row r="105" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
+      <c r="A105" s="13"/>
       <c r="E105" s="4"/>
       <c r="J105" s="6"/>
       <c r="K105" s="6"/>
@@ -1961,7 +1972,7 @@
       <c r="P105" s="9"/>
     </row>
     <row r="106" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
+      <c r="A106" s="13"/>
       <c r="E106" s="4"/>
       <c r="J106" s="6"/>
       <c r="K106" s="6"/>
@@ -1970,14 +1981,14 @@
       <c r="P106" s="9"/>
     </row>
     <row r="107" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
+      <c r="A107" s="13"/>
       <c r="E107" s="4"/>
       <c r="J107" s="6"/>
       <c r="K107" s="6"/>
       <c r="N107" s="7"/>
     </row>
     <row r="108" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
+      <c r="A108" s="13"/>
       <c r="E108" s="4"/>
       <c r="J108" s="6"/>
       <c r="K108" s="6"/>
@@ -1986,14 +1997,14 @@
       <c r="P108" s="9"/>
     </row>
     <row r="109" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
+      <c r="A109" s="13"/>
       <c r="E109" s="4"/>
       <c r="J109" s="6"/>
       <c r="K109" s="6"/>
       <c r="N109" s="7"/>
     </row>
     <row r="110" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
+      <c r="A110" s="13"/>
       <c r="E110" s="4"/>
       <c r="J110" s="6"/>
       <c r="K110" s="6"/>
@@ -2002,7 +2013,7 @@
       <c r="P110" s="9"/>
     </row>
     <row r="111" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
+      <c r="A111" s="13"/>
       <c r="E111" s="4"/>
       <c r="J111" s="6"/>
       <c r="K111" s="6"/>
@@ -2011,28 +2022,28 @@
       <c r="P111" s="9"/>
     </row>
     <row r="112" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
+      <c r="A112" s="13"/>
       <c r="E112" s="4"/>
       <c r="J112" s="6"/>
       <c r="K112" s="6"/>
       <c r="N112" s="7"/>
     </row>
     <row r="113" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
+      <c r="A113" s="13"/>
       <c r="E113" s="4"/>
       <c r="J113" s="6"/>
       <c r="K113" s="6"/>
       <c r="N113" s="7"/>
     </row>
     <row r="114" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="4"/>
+      <c r="A114" s="13"/>
       <c r="E114" s="4"/>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
       <c r="N114" s="7"/>
     </row>
     <row r="115" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="4"/>
+      <c r="A115" s="13"/>
       <c r="E115" s="4"/>
       <c r="J115" s="6"/>
       <c r="K115" s="6"/>
@@ -2041,7 +2052,7 @@
       <c r="P115" s="9"/>
     </row>
     <row r="116" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="4"/>
+      <c r="A116" s="13"/>
       <c r="E116" s="13"/>
       <c r="J116" s="6"/>
       <c r="K116" s="6"/>
@@ -2050,7 +2061,7 @@
       <c r="P116" s="9"/>
     </row>
     <row r="117" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="4"/>
+      <c r="A117" s="13"/>
       <c r="E117" s="4"/>
       <c r="J117" s="6"/>
       <c r="K117" s="6"/>

</xml_diff>